<commit_message>
Update project: Fixed frontend startup issues and added bcrypt authentication improvements
</commit_message>
<xml_diff>
--- a/backend/user_activity_log.xlsx
+++ b/backend/user_activity_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
   <si>
     <t>Timestamp</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>2025-12-22 10:57:49</t>
+  </si>
+  <si>
+    <t>2025-12-26 18:35:33</t>
+  </si>
+  <si>
+    <t>2025-12-28 16:09:04</t>
+  </si>
+  <si>
+    <t>2025-12-28 16:15:25</t>
   </si>
   <si>
     <t>manikandaa944@gmail.com</t>
@@ -449,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,13 +483,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -488,13 +497,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -502,13 +511,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -516,13 +525,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -530,13 +539,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -544,13 +553,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -558,13 +567,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -572,13 +581,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -586,13 +595,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -600,13 +609,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -614,13 +623,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -628,13 +637,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -642,13 +651,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,13 +665,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -670,13 +679,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -684,13 +693,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -698,13 +707,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -712,13 +721,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -726,13 +735,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -740,13 +749,55 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="D21" t="s">
-        <v>24</v>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>